<commit_message>
update label form input
</commit_message>
<xml_diff>
--- a/doc/Tabel Referensi by Walid.xlsx
+++ b/doc/Tabel Referensi by Walid.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4560" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4560" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="source" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="390">
   <si>
     <t>No.</t>
   </si>
@@ -2419,8 +2419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F25"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2432,7 +2432,10 @@
       <c r="A1" t="s">
         <v>138</v>
       </c>
-      <c r="B1">
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1">
         <v>3</v>
       </c>
       <c r="D1" t="str">
@@ -2440,15 +2443,18 @@
         <v>d3akt</v>
       </c>
       <c r="F1" t="str">
-        <f>"&lt;option value='"&amp;B1&amp;D1&amp;"' class='"&amp;D1&amp;"'&gt;"&amp;B1&amp;"&lt;/option&gt;"</f>
-        <v>&lt;option value='3d3akt' class='d3akt'&gt;3&lt;/option&gt;</v>
+        <f>"&lt;option value='"&amp;C1&amp;D1&amp;"' class='"&amp;D1&amp;"'&gt;"&amp;B1&amp;"&lt;/option&gt;"</f>
+        <v>&lt;option value='3d3akt' class='d3akt'&gt;III&lt;/option&gt;</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>138</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
         <v>5</v>
       </c>
       <c r="D2" t="str">
@@ -2456,15 +2462,18 @@
         <v>d3akt</v>
       </c>
       <c r="F2" t="str">
-        <f t="shared" ref="F2:F25" si="0">"&lt;option value='"&amp;B2&amp;D2&amp;"' class='"&amp;D2&amp;"'&gt;"&amp;B2&amp;"&lt;/option&gt;"</f>
-        <v>&lt;option value='5d3akt' class='d3akt'&gt;5&lt;/option&gt;</v>
+        <f t="shared" ref="F2:F25" si="0">"&lt;option value='"&amp;C2&amp;D2&amp;"' class='"&amp;D2&amp;"'&gt;"&amp;B2&amp;"&lt;/option&gt;"</f>
+        <v>&lt;option value='5d3akt' class='d3akt'&gt;V&lt;/option&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>139</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
         <v>3</v>
       </c>
       <c r="D3" t="str">
@@ -2473,14 +2482,17 @@
       </c>
       <c r="F3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value='3d3aktap' class='d3aktap'&gt;3&lt;/option&gt;</v>
+        <v>&lt;option value='3d3aktap' class='d3aktap'&gt;III&lt;/option&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>139</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
         <v>5</v>
       </c>
       <c r="D4" t="str">
@@ -2489,14 +2501,17 @@
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value='5d3aktap' class='d3aktap'&gt;5&lt;/option&gt;</v>
+        <v>&lt;option value='5d3aktap' class='d3aktap'&gt;V&lt;/option&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>149</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5">
         <v>7</v>
       </c>
       <c r="D5" t="str">
@@ -2505,14 +2520,17 @@
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value='7d4aktreg' class='d4aktreg'&gt;7&lt;/option&gt;</v>
+        <v>&lt;option value='7d4aktreg' class='d4aktreg'&gt;VII&lt;/option&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>150</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6">
         <v>7</v>
       </c>
       <c r="D6" t="str">
@@ -2521,14 +2539,17 @@
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value='7d4aktapnonakt' class='d4aktapnonakt'&gt;7&lt;/option&gt;</v>
+        <v>&lt;option value='7d4aktapnonakt' class='d4aktapnonakt'&gt;VII&lt;/option&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>150</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7">
         <v>9</v>
       </c>
       <c r="D7" t="str">
@@ -2537,14 +2558,17 @@
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value='9d4aktapnonakt' class='d4aktapnonakt'&gt;9&lt;/option&gt;</v>
+        <v>&lt;option value='9d4aktapnonakt' class='d4aktapnonakt'&gt;IX&lt;/option&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>140</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="str">
@@ -2553,14 +2577,17 @@
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value='1d3pjk' class='d3pjk'&gt;1&lt;/option&gt;</v>
+        <v>&lt;option value='1d3pjk' class='d3pjk'&gt;I&lt;/option&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>140</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
         <v>3</v>
       </c>
       <c r="D9" t="str">
@@ -2569,14 +2596,17 @@
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value='3d3pjk' class='d3pjk'&gt;3&lt;/option&gt;</v>
+        <v>&lt;option value='3d3pjk' class='d3pjk'&gt;III&lt;/option&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>140</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
         <v>5</v>
       </c>
       <c r="D10" t="str">
@@ -2585,14 +2615,17 @@
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value='5d3pjk' class='d3pjk'&gt;5&lt;/option&gt;</v>
+        <v>&lt;option value='5d3pjk' class='d3pjk'&gt;V&lt;/option&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>141</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
         <v>3</v>
       </c>
       <c r="D11" t="str">
@@ -2601,14 +2634,17 @@
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value='3d3pjkap' class='d3pjkap'&gt;3&lt;/option&gt;</v>
+        <v>&lt;option value='3d3pjkap' class='d3pjkap'&gt;III&lt;/option&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>141</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
         <v>5</v>
       </c>
       <c r="D12" t="str">
@@ -2617,14 +2653,17 @@
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value='5d3pjkap' class='d3pjkap'&gt;5&lt;/option&gt;</v>
+        <v>&lt;option value='5d3pjkap' class='d3pjkap'&gt;V&lt;/option&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>142</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
         <v>3</v>
       </c>
       <c r="D13" t="str">
@@ -2633,14 +2672,17 @@
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value='3d3pbb' class='d3pbb'&gt;3&lt;/option&gt;</v>
+        <v>&lt;option value='3d3pbb' class='d3pbb'&gt;III&lt;/option&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>142</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14">
         <v>5</v>
       </c>
       <c r="D14" t="str">
@@ -2649,14 +2691,17 @@
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value='5d3pbb' class='d3pbb'&gt;5&lt;/option&gt;</v>
+        <v>&lt;option value='5d3pbb' class='d3pbb'&gt;V&lt;/option&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>143</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15">
         <v>4</v>
       </c>
       <c r="D15" t="str">
@@ -2665,14 +2710,17 @@
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value='4d3pbbap' class='d3pbbap'&gt;4&lt;/option&gt;</v>
+        <v>&lt;option value='4d3pbbap' class='d3pbbap'&gt;IV&lt;/option&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>143</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16">
         <v>5</v>
       </c>
       <c r="D16" t="str">
@@ -2681,14 +2729,17 @@
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value='5d3pbbap' class='d3pbbap'&gt;5&lt;/option&gt;</v>
+        <v>&lt;option value='5d3pbbap' class='d3pbbap'&gt;V&lt;/option&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>143</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17">
         <v>6</v>
       </c>
       <c r="D17" t="str">
@@ -2697,14 +2748,17 @@
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value='6d3pbbap' class='d3pbbap'&gt;6&lt;/option&gt;</v>
+        <v>&lt;option value='6d3pbbap' class='d3pbbap'&gt;VI&lt;/option&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>144</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18">
         <v>3</v>
       </c>
       <c r="D18" t="str">
@@ -2713,14 +2767,17 @@
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value='3d3bc' class='d3bc'&gt;3&lt;/option&gt;</v>
+        <v>&lt;option value='3d3bc' class='d3bc'&gt;III&lt;/option&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>144</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19">
         <v>5</v>
       </c>
       <c r="D19" t="str">
@@ -2729,14 +2786,17 @@
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value='5d3bc' class='d3bc'&gt;5&lt;/option&gt;</v>
+        <v>&lt;option value='5d3bc' class='d3bc'&gt;V&lt;/option&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>145</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20">
         <v>5</v>
       </c>
       <c r="D20" t="str">
@@ -2745,14 +2805,17 @@
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value='5d3bcap' class='d3bcap'&gt;5&lt;/option&gt;</v>
+        <v>&lt;option value='5d3bcap' class='d3bcap'&gt;V&lt;/option&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>146</v>
       </c>
-      <c r="B21">
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21">
         <v>3</v>
       </c>
       <c r="D21" t="str">
@@ -2761,14 +2824,17 @@
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value='3d3kbn' class='d3kbn'&gt;3&lt;/option&gt;</v>
+        <v>&lt;option value='3d3kbn' class='d3kbn'&gt;III&lt;/option&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>146</v>
       </c>
-      <c r="B22">
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22">
         <v>5</v>
       </c>
       <c r="D22" t="str">
@@ -2777,14 +2843,17 @@
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value='5d3kbn' class='d3kbn'&gt;5&lt;/option&gt;</v>
+        <v>&lt;option value='5d3kbn' class='d3kbn'&gt;V&lt;/option&gt;</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>147</v>
       </c>
-      <c r="B23">
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23">
         <v>5</v>
       </c>
       <c r="D23" t="str">
@@ -2793,14 +2862,17 @@
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value='5d3kbnap' class='d3kbnap'&gt;5&lt;/option&gt;</v>
+        <v>&lt;option value='5d3kbnap' class='d3kbnap'&gt;V&lt;/option&gt;</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>148</v>
       </c>
-      <c r="B24">
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24">
         <v>3</v>
       </c>
       <c r="D24" t="str">
@@ -2809,14 +2881,17 @@
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value='3d3ma' class='d3ma'&gt;3&lt;/option&gt;</v>
+        <v>&lt;option value='3d3ma' class='d3ma'&gt;III&lt;/option&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>148</v>
       </c>
-      <c r="B25">
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25">
         <v>5</v>
       </c>
       <c r="D25" t="str">
@@ -2825,7 +2900,7 @@
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;option value='5d3ma' class='d3ma'&gt;5&lt;/option&gt;</v>
+        <v>&lt;option value='5d3ma' class='d3ma'&gt;V&lt;/option&gt;</v>
       </c>
     </row>
   </sheetData>
@@ -2837,8 +2912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B135" workbookViewId="0">
-      <selection activeCell="E145" sqref="E145"/>
+    <sheetView topLeftCell="B135" workbookViewId="0">
+      <selection activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>